<commit_message>
change figure labels according to manuscript
</commit_message>
<xml_diff>
--- a/Results/Gene_lists_and_features/Supplementary_table4_burdenanalysiscombinations.xlsx
+++ b/Results/Gene_lists_and_features/Supplementary_table4_burdenanalysiscombinations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z Chen\Documents\PhD Year 3\ataxia_paper\Tables\Final_submission_supp_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z Chen\Documents\PhD Year 3\ataxia_paper\Brain_revision\Supplementary_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36155906-91B1-4C50-A156-426F0246A1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751FD832-DF04-415F-967C-1B0C74FE71C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7764D91A-693D-49B5-87F6-35070013C3C1}"/>
+    <workbookView xWindow="3234" yWindow="3234" windowWidth="17280" windowHeight="9048" xr2:uid="{7764D91A-693D-49B5-87F6-35070013C3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary_table_4" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>n = 3720</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Variants in genes tested</t>
   </si>
@@ -65,15 +62,6 @@
   </si>
   <si>
     <t>Childhood-onset ataxia patients (n = 306)</t>
-  </si>
-  <si>
-    <t>n = 3721</t>
-  </si>
-  <si>
-    <t>n = 3722</t>
-  </si>
-  <si>
-    <t>n = 3723</t>
   </si>
   <si>
     <t xml:space="preserve">Supplementary Table 4 - Summary of four different burden analyses combinations. </t>
@@ -460,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEEDE53-B0C2-4764-A9FE-35383BBE8E49}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.6"/>
@@ -475,7 +463,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -486,16 +474,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.6">
@@ -503,13 +491,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>6658</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.6">
@@ -517,13 +505,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6658</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.6">
@@ -531,13 +519,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
+      <c r="D6" s="4">
+        <v>6658</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.6">
@@ -545,13 +533,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>6658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>